<commit_message>
working 2 testcases of create customer and login
</commit_message>
<xml_diff>
--- a/TestData/CreateAccount.xlsx
+++ b/TestData/CreateAccount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\New Workspace\AkshayFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA2305A-54FC-468E-965B-FD0D32ED5137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332E56F8-A63B-463B-B3EF-782032E65270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,16 +42,16 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>Akshay</t>
-  </si>
-  <si>
-    <t>Metakari</t>
-  </si>
-  <si>
-    <t>ak512@gmail.com</t>
-  </si>
-  <si>
     <t>Heoo12334</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ak1217@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,19 +414,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>